<commit_message>
normalize included in nmf
</commit_message>
<xml_diff>
--- a/Project_python/out/Top2vec/test_top2vec_abstractsHigh0.xlsx
+++ b/Project_python/out/Top2vec/test_top2vec_abstractsHigh0.xlsx
@@ -655,12 +655,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.242|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.250|x11: 0.000|x12: 0.203|x13: 0.305|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.149|x3: 0.053|x4: 0.000|x5: 0.057|x6: 0.055|x7: 0.000|x8: 0.000|x9: 0.065|x10: 0.154|x11: 0.074|x12: 0.124|x13: 0.188|x14: 0.000|x15: 0.082|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.31]</t>
+          <t>[0.00, 0.06, 0.19]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -696,12 +696,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.136|x3: 0.089|x4: 0.047|x5: 0.080|x6: 0.081|x7: 0.000|x8: 0.064|x9: 0.064|x10: 0.101|x11: 0.072|x12: 0.050|x13: 0.095|x14: 0.000|x15: 0.079|x16: 0.043|x17: 0.000</t>
+          <t>x1: 0.031|x2: 0.128|x3: 0.084|x4: 0.044|x5: 0.075|x6: 0.076|x7: 0.028|x8: 0.060|x9: 0.060|x10: 0.095|x11: 0.068|x12: 0.047|x13: 0.089|x14: 0.000|x15: 0.074|x16: 0.041|x17: 0.000</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.14]</t>
+          <t>[0.00, 0.06, 0.13]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -737,12 +737,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>x1: 0.094|x2: 0.000|x3: 0.083|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.242|x10: 0.133|x11: 0.263|x12: 0.088|x13: 0.098|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.076|x2: 0.000|x3: 0.067|x4: 0.000|x5: 0.051|x6: 0.037|x7: 0.000|x8: 0.049|x9: 0.195|x10: 0.107|x11: 0.212|x12: 0.071|x13: 0.079|x14: 0.000|x15: 0.056|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.26]</t>
+          <t>[0.00, 0.06, 0.21]</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -778,7 +778,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>x1: 0.050|x2: 0.079|x3: 0.094|x4: 0.056|x5: 0.072|x6: 0.067|x7: 0.044|x8: 0.063|x9: 0.101|x10: 0.083|x11: 0.095|x12: 0.051|x13: 0.054|x14: 0.000|x15: 0.058|x16: 0.032|x17: 0.000</t>
+          <t>x1: 0.050|x2: 0.078|x3: 0.093|x4: 0.055|x5: 0.071|x6: 0.066|x7: 0.043|x8: 0.063|x9: 0.099|x10: 0.081|x11: 0.094|x12: 0.050|x13: 0.054|x14: 0.014|x15: 0.057|x16: 0.032|x17: 0.000</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -983,12 +983,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.167|x4: 0.084|x5: 0.100|x6: 0.066|x7: 0.000|x8: 0.096|x9: 0.126|x10: 0.100|x11: 0.072|x12: 0.089|x13: 0.000|x14: 0.100|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.043|x2: 0.000|x3: 0.139|x4: 0.070|x5: 0.083|x6: 0.055|x7: 0.044|x8: 0.080|x9: 0.105|x10: 0.083|x11: 0.060|x12: 0.074|x13: 0.047|x14: 0.083|x15: 0.000|x16: 0.032|x17: 0.000</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.17]</t>
+          <t>[0.00, 0.06, 0.14]</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1065,29 +1065,29 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.605|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.395|x17: 0.000</t>
+          <t>x1: 0.071|x2: 0.090|x3: 0.227|x4: 0.000|x5: 0.066|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.064|x11: 0.068|x12: 0.104|x13: 0.097|x14: 0.065|x15: 0.000|x16: 0.148|x17: 0.000</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.61]</t>
+          <t>[0.00, 0.06, 0.23]</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>[0.6054459359560356]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.078|x3: 0.083|x4: 0.057|x5: 0.087|x6: 0.091|x7: 0.040|x8: 0.070|x9: 0.070|x10: 0.079|x11: 0.103|x12: 0.096|x13: 0.033|x14: 0.000|x15: 0.037|x16: 0.075|x17: 0.000</t>
+          <t>x1: 0.013|x2: 0.077|x3: 0.082|x4: 0.056|x5: 0.085|x6: 0.090|x7: 0.039|x8: 0.070|x9: 0.069|x10: 0.078|x11: 0.101|x12: 0.095|x13: 0.033|x14: 0.000|x15: 0.036|x16: 0.074|x17: 0.000</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1147,7 +1147,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>x1: 0.033|x2: 0.035|x3: 0.093|x4: 0.053|x5: 0.089|x6: 0.094|x7: 0.031|x8: 0.101|x9: 0.119|x10: 0.119|x11: 0.082|x12: 0.071|x13: 0.052|x14: 0.000|x15: 0.028|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.032|x2: 0.035|x3: 0.092|x4: 0.052|x5: 0.087|x6: 0.093|x7: 0.030|x8: 0.099|x9: 0.117|x10: 0.117|x11: 0.081|x12: 0.070|x13: 0.051|x14: 0.000|x15: 0.028|x16: 0.018|x17: 0.000</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1188,12 +1188,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.178|x3: 0.371|x4: 0.147|x5: 0.140|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.165|x17: 0.000</t>
+          <t>x1: 0.090|x2: 0.125|x3: 0.260|x4: 0.103|x5: 0.098|x6: 0.000|x7: 0.055|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.080|x15: 0.074|x16: 0.115|x17: 0.000</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.37]</t>
+          <t>[0.00, 0.06, 0.26]</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1229,22 +1229,22 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.575|x12: 0.425|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.180|x10: 0.000|x11: 0.381|x12: 0.282|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.157|x17: 0.000</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.57]</t>
+          <t>[0.00, 0.06, 0.38]</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>[11]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>[0.5747309080116411]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H20" t="b">
@@ -1270,22 +1270,22 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 1.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.135|x4: 0.122|x5: 0.105|x6: 0.085|x7: 0.072|x8: 0.105|x9: 0.000|x10: 0.000|x11: 0.085|x12: 0.104|x13: 0.000|x14: 0.187|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 1.00]</t>
+          <t>[0.00, 0.06, 0.19]</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>[14]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>[1.0]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H21" t="b">
@@ -1311,22 +1311,22 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.513|x9: 0.487|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.208|x4: 0.000|x5: 0.108|x6: 0.000|x7: 0.000|x8: 0.264|x9: 0.250|x10: 0.170|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.51]</t>
+          <t>[0.00, 0.06, 0.26]</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>[0.5128552508743563]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H22" t="b">
@@ -1352,12 +1352,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>x1: 0.086|x2: 0.052|x3: 0.143|x4: 0.086|x5: 0.090|x6: 0.074|x7: 0.073|x8: 0.068|x9: 0.084|x10: 0.054|x11: 0.082|x12: 0.000|x13: 0.000|x14: 0.055|x15: 0.053|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.078|x2: 0.047|x3: 0.131|x4: 0.078|x5: 0.082|x6: 0.067|x7: 0.067|x8: 0.062|x9: 0.077|x10: 0.050|x11: 0.075|x12: 0.044|x13: 0.000|x14: 0.050|x15: 0.049|x16: 0.044|x17: 0.000</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.14]</t>
+          <t>[0.00, 0.06, 0.13]</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.044|x3: 0.106|x4: 0.064|x5: 0.114|x6: 0.103|x7: 0.053|x8: 0.095|x9: 0.082|x10: 0.093|x11: 0.075|x12: 0.082|x13: 0.032|x14: 0.000|x15: 0.000|x16: 0.056|x17: 0.000</t>
+          <t>x1: 0.017|x2: 0.042|x3: 0.102|x4: 0.061|x5: 0.110|x6: 0.099|x7: 0.051|x8: 0.091|x9: 0.079|x10: 0.089|x11: 0.073|x12: 0.079|x13: 0.031|x14: 0.000|x15: 0.022|x16: 0.054|x17: 0.000</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1434,7 +1434,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.058|x3: 0.083|x4: 0.051|x5: 0.100|x6: 0.103|x7: 0.037|x8: 0.101|x9: 0.086|x10: 0.113|x11: 0.072|x12: 0.068|x13: 0.053|x14: 0.000|x15: 0.034|x16: 0.041|x17: 0.000</t>
+          <t>x1: 0.017|x2: 0.057|x3: 0.082|x4: 0.050|x5: 0.098|x6: 0.101|x7: 0.036|x8: 0.099|x9: 0.085|x10: 0.111|x11: 0.071|x12: 0.067|x13: 0.052|x14: 0.000|x15: 0.034|x16: 0.041|x17: 0.000</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1475,12 +1475,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>x1: 0.266|x2: 0.000|x3: 0.463|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.271|x17: 0.000</t>
+          <t>x1: 0.172|x2: 0.000|x3: 0.300|x4: 0.071|x5: 0.079|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.058|x12: 0.076|x13: 0.000|x14: 0.000|x15: 0.069|x16: 0.175|x17: 0.000</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.46]</t>
+          <t>[0.00, 0.06, 0.30]</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1598,12 +1598,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.185|x4: 0.000|x5: 0.236|x6: 0.188|x7: 0.000|x8: 0.146|x9: 0.000|x10: 0.131|x11: 0.000|x12: 0.115|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.034|x3: 0.141|x4: 0.040|x5: 0.180|x6: 0.143|x7: 0.000|x8: 0.111|x9: 0.055|x10: 0.100|x11: 0.036|x12: 0.087|x13: 0.036|x14: 0.000|x15: 0.000|x16: 0.037|x17: 0.000</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.24]</t>
+          <t>[0.00, 0.06, 0.18]</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1639,12 +1639,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>x1: 0.091|x2: 0.071|x3: 0.186|x4: 0.054|x5: 0.075|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.075|x10: 0.000|x11: 0.111|x12: 0.077|x13: 0.000|x14: 0.129|x15: 0.065|x16: 0.067|x17: 0.000</t>
+          <t>x1: 0.080|x2: 0.062|x3: 0.163|x4: 0.047|x5: 0.066|x6: 0.035|x7: 0.000|x8: 0.022|x9: 0.066|x10: 0.037|x11: 0.097|x12: 0.067|x13: 0.029|x14: 0.113|x15: 0.057|x16: 0.059|x17: 0.000</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.19]</t>
+          <t>[0.00, 0.06, 0.16]</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1680,12 +1680,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>x1: 0.099|x2: 0.066|x3: 0.199|x4: 0.066|x5: 0.078|x6: 0.000|x7: 0.049|x8: 0.043|x9: 0.050|x10: 0.000|x11: 0.066|x12: 0.047|x13: 0.000|x14: 0.076|x15: 0.056|x16: 0.105|x17: 0.000</t>
+          <t>x1: 0.095|x2: 0.063|x3: 0.189|x4: 0.063|x5: 0.074|x6: 0.029|x7: 0.047|x8: 0.041|x9: 0.048|x10: 0.019|x11: 0.063|x12: 0.045|x13: 0.000|x14: 0.072|x15: 0.053|x16: 0.100|x17: 0.000</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.20]</t>
+          <t>[0.00, 0.06, 0.19]</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1762,12 +1762,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>x1: 0.072|x2: 0.000|x3: 0.162|x4: 0.057|x5: 0.073|x6: 0.063|x7: 0.000|x8: 0.083|x9: 0.104|x10: 0.077|x11: 0.075|x12: 0.075|x13: 0.000|x14: 0.096|x15: 0.000|x16: 0.062|x17: 0.000</t>
+          <t>x1: 0.063|x2: 0.030|x3: 0.143|x4: 0.050|x5: 0.064|x6: 0.056|x7: 0.025|x8: 0.074|x9: 0.092|x10: 0.068|x11: 0.066|x12: 0.067|x13: 0.028|x14: 0.085|x15: 0.032|x16: 0.055|x17: 0.000</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.16]</t>
+          <t>[0.00, 0.06, 0.14]</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1803,22 +1803,22 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 1.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.305|x10: 0.212|x11: 0.484|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 1.00]</t>
+          <t>[0.00, 0.06, 0.48]</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>[11]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>[1.0]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H34" t="b">
@@ -1844,12 +1844,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>x1: 0.139|x2: 0.000|x3: 0.218|x4: 0.000|x5: 0.076|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.146|x12: 0.094|x13: 0.000|x14: 0.080|x15: 0.075|x16: 0.172|x17: 0.000</t>
+          <t>x1: 0.131|x2: 0.000|x3: 0.204|x4: 0.062|x5: 0.072|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.137|x12: 0.088|x13: 0.000|x14: 0.075|x15: 0.070|x16: 0.161|x17: 0.000</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.22]</t>
+          <t>[0.00, 0.06, 0.20]</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1885,7 +1885,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>x1: 0.074|x2: 0.067|x3: 0.173|x4: 0.080|x5: 0.091|x6: 0.051|x7: 0.054|x8: 0.052|x9: 0.066|x10: 0.000|x11: 0.056|x12: 0.045|x13: 0.000|x14: 0.092|x15: 0.050|x16: 0.049|x17: 0.000</t>
+          <t>x1: 0.072|x2: 0.065|x3: 0.168|x4: 0.078|x5: 0.089|x6: 0.049|x7: 0.053|x8: 0.050|x9: 0.064|x10: 0.030|x11: 0.055|x12: 0.044|x13: 0.000|x14: 0.089|x15: 0.048|x16: 0.048|x17: 0.000</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1926,22 +1926,22 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 1.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[nan, nan, nan]</t>
+          <t>[0.00, 0.06, 1.00]</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[11]</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[1.0]</t>
         </is>
       </c>
       <c r="H37" t="b">
@@ -1967,12 +1967,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>x1: 0.093|x2: 0.000|x3: 0.218|x4: 0.000|x5: 0.084|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.071|x10: 0.067|x11: 0.127|x12: 0.123|x13: 0.000|x14: 0.067|x15: 0.000|x16: 0.150|x17: 0.000</t>
+          <t>x1: 0.073|x2: 0.029|x3: 0.171|x4: 0.047|x5: 0.066|x6: 0.040|x7: 0.000|x8: 0.039|x9: 0.056|x10: 0.052|x11: 0.100|x12: 0.097|x13: 0.034|x14: 0.053|x15: 0.028|x16: 0.118|x17: 0.000</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.22]</t>
+          <t>[0.00, 0.06, 0.17]</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2008,12 +2008,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>x1: 0.091|x2: 0.079|x3: 0.183|x4: 0.066|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.165|x12: 0.130|x13: 0.000|x14: 0.000|x15: 0.062|x16: 0.225|x17: 0.000</t>
+          <t>x1: 0.075|x2: 0.065|x3: 0.150|x4: 0.054|x5: 0.044|x6: 0.029|x7: 0.000|x8: 0.028|x9: 0.035|x10: 0.000|x11: 0.136|x12: 0.107|x13: 0.000|x14: 0.040|x15: 0.051|x16: 0.186|x17: 0.000</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.23]</t>
+          <t>[0.00, 0.06, 0.19]</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2049,12 +2049,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>x1: 0.125|x2: 0.081|x3: 0.247|x4: 0.078|x5: 0.080|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.059|x12: 0.090|x13: 0.000|x14: 0.000|x15: 0.079|x16: 0.159|x17: 0.000</t>
+          <t>x1: 0.113|x2: 0.073|x3: 0.223|x4: 0.071|x5: 0.072|x6: 0.000|x7: 0.026|x8: 0.000|x9: 0.031|x10: 0.000|x11: 0.054|x12: 0.081|x13: 0.000|x14: 0.041|x15: 0.071|x16: 0.144|x17: 0.000</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.25]</t>
+          <t>[0.00, 0.06, 0.22]</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2131,22 +2131,22 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.459|x10: 0.000|x11: 0.541|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>[nan, nan, nan]</t>
+          <t>[0.00, 0.06, 0.54]</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[11]</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[0.5411625943438155]</t>
         </is>
       </c>
       <c r="H42" t="b">
@@ -2172,29 +2172,29 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.454|x10: 0.000|x11: 0.546|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>[nan, nan, nan]</t>
+          <t>[0.00, 0.06, 0.55]</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[11]</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[0.5459981812760496]</t>
         </is>
       </c>
       <c r="H43" t="b">
         <v>0</v>
       </c>
       <c r="I43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>x1: 0.097|x2: 0.052|x3: 0.171|x4: 0.046|x5: 0.066|x6: 0.043|x7: 0.038|x8: 0.053|x9: 0.081|x10: 0.035|x11: 0.081|x12: 0.045|x13: 0.000|x14: 0.056|x15: 0.051|x16: 0.086|x17: 0.000</t>
+          <t>x1: 0.095|x2: 0.052|x3: 0.169|x4: 0.046|x5: 0.064|x6: 0.043|x7: 0.037|x8: 0.052|x9: 0.080|x10: 0.034|x11: 0.080|x12: 0.044|x13: 0.017|x14: 0.055|x15: 0.050|x16: 0.084|x17: 0.000</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2254,12 +2254,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.228|x4: 0.000|x5: 0.000|x6: 0.231|x7: 0.000|x8: 0.287|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.254|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.129|x4: 0.000|x5: 0.065|x6: 0.130|x7: 0.064|x8: 0.162|x9: 0.113|x10: 0.103|x11: 0.000|x12: 0.091|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.143|x17: 0.000</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.29]</t>
+          <t>[0.00, 0.06, 0.16]</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2295,12 +2295,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>x1: 0.098|x2: 0.071|x3: 0.148|x4: 0.102|x5: 0.090|x6: 0.075|x7: 0.099|x8: 0.066|x9: 0.065|x10: 0.000|x11: 0.057|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.069|x16: 0.059|x17: 0.000</t>
+          <t>x1: 0.090|x2: 0.065|x3: 0.136|x4: 0.094|x5: 0.083|x6: 0.069|x7: 0.091|x8: 0.061|x9: 0.059|x10: 0.036|x11: 0.052|x12: 0.000|x13: 0.000|x14: 0.049|x15: 0.063|x16: 0.054|x17: 0.000</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.15]</t>
+          <t>[0.00, 0.06, 0.14]</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2336,12 +2336,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.219|x3: 0.265|x4: 0.248|x5: 0.140|x6: 0.000|x7: 0.128|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.198|x3: 0.239|x4: 0.224|x5: 0.127|x6: 0.047|x7: 0.115|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.050|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.26]</t>
+          <t>[0.00, 0.06, 0.24]</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2377,12 +2377,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>x1: 0.138|x2: 0.171|x3: 0.191|x4: 0.124|x5: 0.000|x6: 0.078|x7: 0.000|x8: 0.000|x9: 0.078|x10: 0.000|x11: 0.105|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.115|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.101|x2: 0.125|x3: 0.140|x4: 0.090|x5: 0.053|x6: 0.057|x7: 0.035|x8: 0.036|x9: 0.057|x10: 0.032|x11: 0.077|x12: 0.031|x13: 0.000|x14: 0.044|x15: 0.084|x16: 0.038|x17: 0.000</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.19]</t>
+          <t>[0.00, 0.06, 0.14]</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2418,12 +2418,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.182|x3: 0.182|x4: 0.177|x5: 0.122|x6: 0.082|x7: 0.102|x8: 0.094|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.059|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.158|x3: 0.158|x4: 0.154|x5: 0.106|x6: 0.071|x7: 0.088|x8: 0.081|x9: 0.038|x10: 0.000|x11: 0.036|x12: 0.029|x13: 0.000|x14: 0.051|x15: 0.028|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.18]</t>
+          <t>[0.00, 0.06, 0.16]</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2459,22 +2459,22 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.479|x3: 0.521|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.138|x2: 0.204|x3: 0.223|x4: 0.144|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.085|x12: 0.000|x13: 0.000|x14: 0.112|x15: 0.093|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.52]</t>
+          <t>[0.00, 0.06, 0.22]</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>[0.5214464195572255]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H50" t="b">
@@ -2500,12 +2500,12 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>x1: 0.047|x2: 0.081|x3: 0.109|x4: 0.088|x5: 0.077|x6: 0.076|x7: 0.050|x8: 0.078|x9: 0.100|x10: 0.089|x11: 0.072|x12: 0.060|x13: 0.030|x14: 0.000|x15: 0.043|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.046|x2: 0.078|x3: 0.105|x4: 0.085|x5: 0.074|x6: 0.074|x7: 0.049|x8: 0.075|x9: 0.096|x10: 0.086|x11: 0.070|x12: 0.058|x13: 0.029|x14: 0.019|x15: 0.042|x16: 0.015|x17: 0.000</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.11]</t>
+          <t>[0.00, 0.06, 0.10]</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2541,12 +2541,12 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.233|x3: 0.292|x4: 0.263|x5: 0.102|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.110|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.201|x3: 0.252|x4: 0.227|x5: 0.088|x6: 0.000|x7: 0.077|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.059|x13: 0.000|x14: 0.095|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.29]</t>
+          <t>[0.00, 0.06, 0.25]</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2582,12 +2582,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.218|x3: 0.220|x4: 0.192|x5: 0.098|x6: 0.000|x7: 0.089|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.096|x12: 0.000|x13: 0.000|x14: 0.087|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.189|x3: 0.191|x4: 0.167|x5: 0.085|x6: 0.000|x7: 0.077|x8: 0.000|x9: 0.043|x10: 0.000|x11: 0.084|x12: 0.051|x13: 0.000|x14: 0.075|x15: 0.038|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.22]</t>
+          <t>[0.00, 0.06, 0.19]</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -2623,12 +2623,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.292|x3: 0.231|x4: 0.160|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.147|x10: 0.000|x11: 0.170|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.272|x3: 0.216|x4: 0.149|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.137|x10: 0.067|x11: 0.159|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.29]</t>
+          <t>[0.00, 0.06, 0.27]</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -2664,12 +2664,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.310|x13: 0.000|x14: 0.690|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.172|x12: 0.257|x13: 0.000|x14: 0.571|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.69]</t>
+          <t>[0.00, 0.06, 0.57]</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2679,7 +2679,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>[0.6899204114424827]</t>
+          <t>[0.5712999079496351]</t>
         </is>
       </c>
       <c r="H55" t="b">
@@ -2746,12 +2746,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.120|x4: 0.111|x5: 0.073|x6: 0.000|x7: 0.084|x8: 0.000|x9: 0.081|x10: 0.000|x11: 0.098|x12: 0.134|x13: 0.000|x14: 0.298|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.051|x3: 0.100|x4: 0.092|x5: 0.061|x6: 0.000|x7: 0.070|x8: 0.039|x9: 0.067|x10: 0.041|x11: 0.082|x12: 0.111|x13: 0.039|x14: 0.247|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.30]</t>
+          <t>[0.00, 0.06, 0.25]</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -2787,12 +2787,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.193|x4: 0.221|x5: 0.181|x6: 0.000|x7: 0.207|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.087|x13: 0.000|x14: 0.111|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.165|x4: 0.189|x5: 0.155|x6: 0.038|x7: 0.178|x8: 0.000|x9: 0.062|x10: 0.000|x11: 0.044|x12: 0.075|x13: 0.000|x14: 0.095|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.22]</t>
+          <t>[0.00, 0.06, 0.19]</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -2828,12 +2828,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.214|x4: 0.226|x5: 0.159|x6: 0.000|x7: 0.146|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.132|x13: 0.000|x14: 0.122|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.060|x3: 0.176|x4: 0.186|x5: 0.130|x6: 0.000|x7: 0.120|x8: 0.000|x9: 0.061|x10: 0.000|x11: 0.058|x12: 0.109|x13: 0.000|x14: 0.100|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.23]</t>
+          <t>[0.00, 0.06, 0.19]</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -2869,12 +2869,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>x1: 0.056|x2: 0.053|x3: 0.166|x4: 0.116|x5: 0.099|x6: 0.039|x7: 0.056|x8: 0.047|x9: 0.050|x10: 0.036|x11: 0.063|x12: 0.051|x13: 0.000|x14: 0.097|x15: 0.038|x16: 0.032|x17: 0.000</t>
+          <t>x1: 0.055|x2: 0.052|x3: 0.163|x4: 0.114|x5: 0.097|x6: 0.038|x7: 0.055|x8: 0.047|x9: 0.049|x10: 0.035|x11: 0.062|x12: 0.050|x13: 0.017|x14: 0.096|x15: 0.037|x16: 0.031|x17: 0.000</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.17]</t>
+          <t>[0.00, 0.06, 0.16]</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2951,12 +2951,12 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>x1: 0.047|x2: 0.046|x3: 0.056|x4: 0.000|x5: 0.056|x6: 0.057|x7: 0.000|x8: 0.074|x9: 0.134|x10: 0.146|x11: 0.106|x12: 0.081|x13: 0.147|x14: 0.000|x15: 0.050|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.045|x2: 0.044|x3: 0.053|x4: 0.023|x5: 0.053|x6: 0.055|x7: 0.023|x8: 0.071|x9: 0.128|x10: 0.140|x11: 0.101|x12: 0.077|x13: 0.140|x14: 0.000|x15: 0.048|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.15]</t>
+          <t>[0.00, 0.06, 0.14]</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -2992,12 +2992,12 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>x1: 0.040|x2: 0.045|x3: 0.116|x4: 0.038|x5: 0.092|x6: 0.077|x7: 0.000|x8: 0.066|x9: 0.129|x10: 0.101|x11: 0.104|x12: 0.095|x13: 0.059|x14: 0.000|x15: 0.037|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.038|x2: 0.042|x3: 0.109|x4: 0.035|x5: 0.086|x6: 0.073|x7: 0.019|x8: 0.063|x9: 0.121|x10: 0.095|x11: 0.098|x12: 0.090|x13: 0.056|x14: 0.018|x15: 0.035|x16: 0.020|x17: 0.000</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.13]</t>
+          <t>[0.00, 0.06, 0.12]</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -3074,7 +3074,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>x1: 0.035|x2: 0.047|x3: 0.098|x4: 0.041|x5: 0.075|x6: 0.080|x7: 0.000|x8: 0.079|x9: 0.132|x10: 0.123|x11: 0.105|x12: 0.068|x13: 0.085|x14: 0.000|x15: 0.032|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.033|x2: 0.045|x3: 0.095|x4: 0.039|x5: 0.072|x6: 0.077|x7: 0.021|x8: 0.075|x9: 0.127|x10: 0.118|x11: 0.101|x12: 0.065|x13: 0.082|x14: 0.000|x15: 0.031|x16: 0.018|x17: 0.000</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -3115,12 +3115,12 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.149|x4: 0.000|x5: 0.146|x6: 0.105|x7: 0.000|x8: 0.081|x9: 0.134|x10: 0.137|x11: 0.088|x12: 0.084|x13: 0.076|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.024|x2: 0.000|x3: 0.138|x4: 0.030|x5: 0.135|x6: 0.097|x7: 0.000|x8: 0.075|x9: 0.123|x10: 0.126|x11: 0.081|x12: 0.077|x13: 0.070|x14: 0.000|x15: 0.024|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.15]</t>
+          <t>[0.00, 0.06, 0.14]</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -3156,7 +3156,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>x1: 0.047|x2: 0.071|x3: 0.074|x4: 0.075|x5: 0.105|x6: 0.101|x7: 0.108|x8: 0.130|x9: 0.091|x10: 0.042|x11: 0.055|x12: 0.026|x13: 0.000|x14: 0.031|x15: 0.045|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.046|x2: 0.069|x3: 0.072|x4: 0.074|x5: 0.103|x6: 0.099|x7: 0.106|x8: 0.128|x9: 0.089|x10: 0.041|x11: 0.054|x12: 0.025|x13: 0.000|x14: 0.030|x15: 0.044|x16: 0.022|x17: 0.000</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -3238,7 +3238,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>x1: 0.070|x2: 0.061|x3: 0.115|x4: 0.091|x5: 0.117|x6: 0.081|x7: 0.121|x8: 0.107|x9: 0.069|x10: 0.030|x11: 0.000|x12: 0.028|x13: 0.000|x14: 0.033|x15: 0.049|x16: 0.028|x17: 0.000</t>
+          <t>x1: 0.069|x2: 0.061|x3: 0.114|x4: 0.090|x5: 0.115|x6: 0.080|x7: 0.119|x8: 0.105|x9: 0.068|x10: 0.030|x11: 0.013|x12: 0.027|x13: 0.000|x14: 0.033|x15: 0.049|x16: 0.028|x17: 0.000</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -3279,12 +3279,12 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>x1: 0.051|x2: 0.000|x3: 0.146|x4: 0.080|x5: 0.153|x6: 0.119|x7: 0.066|x8: 0.100|x9: 0.083|x10: 0.082|x11: 0.060|x12: 0.059|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.047|x2: 0.041|x3: 0.136|x4: 0.074|x5: 0.142|x6: 0.111|x7: 0.061|x8: 0.093|x9: 0.077|x10: 0.076|x11: 0.055|x12: 0.055|x13: 0.000|x14: 0.000|x15: 0.032|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.15]</t>
+          <t>[0.00, 0.06, 0.14]</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -3320,7 +3320,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>x1: 0.060|x2: 0.059|x3: 0.083|x4: 0.083|x5: 0.099|x6: 0.113|x7: 0.083|x8: 0.124|x9: 0.096|x10: 0.081|x11: 0.066|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.053|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.059|x2: 0.057|x3: 0.081|x4: 0.081|x5: 0.097|x6: 0.111|x7: 0.081|x8: 0.121|x9: 0.094|x10: 0.079|x11: 0.064|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.052|x16: 0.022|x17: 0.000</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -3361,7 +3361,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.049|x3: 0.077|x4: 0.074|x5: 0.134|x6: 0.131|x7: 0.079|x8: 0.225|x9: 0.134|x10: 0.097|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.048|x3: 0.075|x4: 0.071|x5: 0.129|x6: 0.127|x7: 0.077|x8: 0.217|x9: 0.129|x10: 0.094|x11: 0.032|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -3402,7 +3402,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>x1: 0.044|x2: 0.052|x3: 0.115|x4: 0.044|x5: 0.092|x6: 0.076|x7: 0.029|x8: 0.076|x9: 0.105|x10: 0.100|x11: 0.072|x12: 0.064|x13: 0.064|x14: 0.000|x15: 0.042|x16: 0.025|x17: 0.000</t>
+          <t>x1: 0.043|x2: 0.051|x3: 0.114|x4: 0.043|x5: 0.091|x6: 0.075|x7: 0.029|x8: 0.075|x9: 0.104|x10: 0.099|x11: 0.072|x12: 0.064|x13: 0.063|x14: 0.012|x15: 0.041|x16: 0.025|x17: 0.000</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -3443,12 +3443,12 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>x1: 0.065|x2: 0.000|x3: 0.094|x4: 0.000|x5: 0.120|x6: 0.138|x7: 0.062|x8: 0.205|x9: 0.171|x10: 0.144|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.057|x2: 0.000|x3: 0.082|x4: 0.039|x5: 0.105|x6: 0.121|x7: 0.055|x8: 0.180|x9: 0.150|x10: 0.127|x11: 0.041|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.043|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.20]</t>
+          <t>[0.00, 0.06, 0.18]</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -3484,12 +3484,12 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>x1: 0.050|x2: 0.069|x3: 0.086|x4: 0.080|x5: 0.108|x6: 0.099|x7: 0.097|x8: 0.126|x9: 0.071|x10: 0.049|x11: 0.038|x12: 0.024|x13: 0.000|x14: 0.031|x15: 0.047|x16: 0.026|x17: 0.000</t>
+          <t>x1: 0.049|x2: 0.068|x3: 0.085|x4: 0.079|x5: 0.106|x6: 0.097|x7: 0.095|x8: 0.124|x9: 0.070|x10: 0.048|x11: 0.037|x12: 0.023|x13: 0.018|x14: 0.030|x15: 0.046|x16: 0.026|x17: 0.000</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.13]</t>
+          <t>[0.00, 0.06, 0.12]</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -3525,12 +3525,12 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 1.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.310|x13: 0.000|x14: 0.690|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 1.00]</t>
+          <t>[0.00, 0.06, 0.69]</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -3540,7 +3540,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>[1.0]</t>
+          <t>[0.6899204114424827]</t>
         </is>
       </c>
       <c r="H76" t="b">
@@ -3566,12 +3566,12 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>x1: 0.041|x2: 0.048|x3: 0.126|x4: 0.094|x5: 0.089|x6: 0.055|x7: 0.079|x8: 0.069|x9: 0.086|x10: 0.049|x11: 0.050|x12: 0.062|x13: 0.031|x14: 0.087|x15: 0.033|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.040|x2: 0.047|x3: 0.123|x4: 0.092|x5: 0.087|x6: 0.054|x7: 0.077|x8: 0.067|x9: 0.084|x10: 0.048|x11: 0.049|x12: 0.061|x13: 0.031|x14: 0.085|x15: 0.032|x16: 0.023|x17: 0.000</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.13]</t>
+          <t>[0.00, 0.06, 0.12]</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -3607,7 +3607,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>x1: 0.051|x2: 0.061|x3: 0.129|x4: 0.126|x5: 0.114|x6: 0.056|x7: 0.131|x8: 0.070|x9: 0.065|x10: 0.000|x11: 0.000|x12: 0.061|x13: 0.000|x14: 0.094|x15: 0.042|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.048|x2: 0.058|x3: 0.123|x4: 0.121|x5: 0.109|x6: 0.053|x7: 0.125|x8: 0.067|x9: 0.062|x10: 0.000|x11: 0.028|x12: 0.058|x13: 0.000|x14: 0.090|x15: 0.040|x16: 0.018|x17: 0.000</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -3648,12 +3648,12 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.290|x9: 0.445|x10: 0.265|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.079|x2: 0.000|x3: 0.073|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.097|x8: 0.185|x9: 0.284|x10: 0.169|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.113|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.44]</t>
+          <t>[0.00, 0.06, 0.28]</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -3689,7 +3689,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>x1: 0.098|x2: 0.057|x3: 0.115|x4: 0.054|x5: 0.067|x6: 0.046|x7: 0.039|x8: 0.064|x9: 0.098|x10: 0.051|x11: 0.099|x12: 0.034|x13: 0.000|x14: 0.075|x15: 0.073|x16: 0.031|x17: 0.000</t>
+          <t>x1: 0.095|x2: 0.055|x3: 0.112|x4: 0.053|x5: 0.066|x6: 0.045|x7: 0.038|x8: 0.062|x9: 0.095|x10: 0.050|x11: 0.096|x12: 0.033|x13: 0.026|x14: 0.073|x15: 0.071|x16: 0.031|x17: 0.000</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -3730,12 +3730,12 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>x1: 0.033|x2: 0.042|x3: 0.088|x4: 0.053|x5: 0.091|x6: 0.095|x7: 0.049|x8: 0.116|x9: 0.102|x10: 0.105|x11: 0.063|x12: 0.059|x13: 0.031|x14: 0.000|x15: 0.031|x16: 0.041|x17: 0.000</t>
+          <t>x1: 0.033|x2: 0.041|x3: 0.086|x4: 0.052|x5: 0.090|x6: 0.094|x7: 0.048|x8: 0.115|x9: 0.100|x10: 0.103|x11: 0.062|x12: 0.058|x13: 0.030|x14: 0.017|x15: 0.031|x16: 0.041|x17: 0.000</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.12]</t>
+          <t>[0.00, 0.06, 0.11]</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -3771,7 +3771,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>x1: 0.053|x2: 0.060|x3: 0.116|x4: 0.078|x5: 0.097|x6: 0.081|x7: 0.074|x8: 0.124|x9: 0.096|x10: 0.074|x11: 0.031|x12: 0.000|x13: 0.000|x14: 0.041|x15: 0.042|x16: 0.035|x17: 0.000</t>
+          <t>x1: 0.051|x2: 0.058|x3: 0.114|x4: 0.076|x5: 0.095|x6: 0.080|x7: 0.072|x8: 0.121|x9: 0.094|x10: 0.073|x11: 0.031|x12: 0.020|x13: 0.000|x14: 0.040|x15: 0.041|x16: 0.034|x17: 0.000</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -3812,12 +3812,12 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>x1: 0.062|x2: 0.062|x3: 0.088|x4: 0.042|x5: 0.075|x6: 0.073|x7: 0.000|x8: 0.089|x9: 0.145|x10: 0.092|x11: 0.133|x12: 0.083|x13: 0.000|x14: 0.000|x15: 0.056|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.057|x2: 0.057|x3: 0.080|x4: 0.039|x5: 0.068|x6: 0.066|x7: 0.028|x8: 0.081|x9: 0.133|x10: 0.084|x11: 0.121|x12: 0.076|x13: 0.032|x14: 0.000|x15: 0.051|x16: 0.027|x17: 0.000</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.15]</t>
+          <t>[0.00, 0.06, 0.13]</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -3853,12 +3853,12 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.213|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.223|x9: 0.302|x10: 0.263|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.134|x4: 0.000|x5: 0.086|x6: 0.000|x7: 0.000|x8: 0.140|x9: 0.190|x10: 0.165|x11: 0.000|x12: 0.074|x13: 0.079|x14: 0.130|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.30]</t>
+          <t>[0.00, 0.06, 0.19]</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -3935,7 +3935,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>x1: 0.042|x2: 0.048|x3: 0.112|x4: 0.045|x5: 0.083|x6: 0.066|x7: 0.031|x8: 0.059|x9: 0.108|x10: 0.094|x11: 0.074|x12: 0.124|x13: 0.049|x14: 0.000|x15: 0.035|x16: 0.032|x17: 0.000</t>
+          <t>x1: 0.041|x2: 0.047|x3: 0.110|x4: 0.044|x5: 0.082|x6: 0.065|x7: 0.030|x8: 0.058|x9: 0.106|x10: 0.092|x11: 0.073|x12: 0.122|x13: 0.048|x14: 0.016|x15: 0.035|x16: 0.031|x17: 0.000</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -3976,12 +3976,12 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>x1: 0.059|x2: 0.051|x3: 0.071|x4: 0.049|x5: 0.071|x6: 0.076|x7: 0.000|x8: 0.096|x9: 0.111|x10: 0.126|x11: 0.125|x12: 0.000|x13: 0.107|x14: 0.000|x15: 0.056|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.052|x2: 0.045|x3: 0.063|x4: 0.044|x5: 0.062|x6: 0.068|x7: 0.029|x8: 0.085|x9: 0.098|x10: 0.112|x11: 0.111|x12: 0.034|x13: 0.094|x14: 0.030|x15: 0.050|x16: 0.022|x17: 0.000</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.13]</t>
+          <t>[0.00, 0.06, 0.11]</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -4017,12 +4017,12 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>x1: 0.212|x2: 0.000|x3: 0.278|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.319|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.191|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.125|x2: 0.000|x3: 0.164|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.100|x9: 0.188|x10: 0.087|x11: 0.092|x12: 0.000|x13: 0.000|x14: 0.113|x15: 0.055|x16: 0.076|x17: 0.000</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.32]</t>
+          <t>[0.00, 0.06, 0.19]</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -4058,12 +4058,12 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.290|x10: 0.000|x11: 0.375|x12: 0.335|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.221|x10: 0.117|x11: 0.285|x12: 0.254|x13: 0.000|x14: 0.123|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.38]</t>
+          <t>[0.00, 0.06, 0.29]</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -4099,7 +4099,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>x1: 0.030|x2: 0.059|x3: 0.070|x4: 0.070|x5: 0.099|x6: 0.115|x7: 0.072|x8: 0.131|x9: 0.094|x10: 0.084|x11: 0.048|x12: 0.040|x13: 0.029|x14: 0.000|x15: 0.039|x16: 0.020|x17: 0.000</t>
+          <t>x1: 0.030|x2: 0.058|x3: 0.069|x4: 0.069|x5: 0.098|x6: 0.114|x7: 0.071|x8: 0.130|x9: 0.093|x10: 0.084|x11: 0.047|x12: 0.040|x13: 0.029|x14: 0.010|x15: 0.038|x16: 0.020|x17: 0.000</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -4140,12 +4140,12 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>x1: 0.071|x2: 0.067|x3: 0.108|x4: 0.060|x5: 0.084|x6: 0.068|x7: 0.043|x8: 0.077|x9: 0.116|x10: 0.079|x11: 0.120|x12: 0.000|x13: 0.044|x14: 0.000|x15: 0.064|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.066|x2: 0.062|x3: 0.100|x4: 0.056|x5: 0.078|x6: 0.063|x7: 0.040|x8: 0.071|x9: 0.108|x10: 0.073|x11: 0.112|x12: 0.025|x13: 0.041|x14: 0.021|x15: 0.060|x16: 0.024|x17: 0.000</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.12]</t>
+          <t>[0.00, 0.06, 0.11]</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -4181,12 +4181,12 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>x1: 0.076|x2: 0.000|x3: 0.119|x4: 0.000|x5: 0.107|x6: 0.097|x7: 0.000|x8: 0.089|x9: 0.139|x10: 0.128|x11: 0.105|x12: 0.139|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.061|x2: 0.026|x3: 0.096|x4: 0.029|x5: 0.086|x6: 0.078|x7: 0.000|x8: 0.072|x9: 0.112|x10: 0.103|x11: 0.085|x12: 0.112|x13: 0.049|x14: 0.043|x15: 0.047|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.14]</t>
+          <t>[0.00, 0.06, 0.11]</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -4222,7 +4222,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>x1: 0.039|x2: 0.050|x3: 0.091|x4: 0.047|x5: 0.073|x6: 0.062|x7: 0.042|x8: 0.054|x9: 0.119|x10: 0.093|x11: 0.071|x12: 0.132|x13: 0.058|x14: 0.028|x15: 0.040|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.038|x2: 0.049|x3: 0.089|x4: 0.046|x5: 0.072|x6: 0.061|x7: 0.041|x8: 0.053|x9: 0.117|x10: 0.092|x11: 0.070|x12: 0.130|x13: 0.057|x14: 0.027|x15: 0.040|x16: 0.017|x17: 0.000</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -4304,7 +4304,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.041|x3: 0.068|x4: 0.031|x5: 0.075|x6: 0.075|x7: 0.034|x8: 0.076|x9: 0.147|x10: 0.127|x11: 0.066|x12: 0.184|x13: 0.075|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.041|x3: 0.067|x4: 0.030|x5: 0.074|x6: 0.074|x7: 0.033|x8: 0.074|x9: 0.145|x10: 0.125|x11: 0.065|x12: 0.181|x13: 0.073|x14: 0.000|x15: 0.017|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -4345,12 +4345,12 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.103|x4: 0.000|x5: 0.093|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.181|x10: 0.131|x11: 0.118|x12: 0.270|x13: 0.104|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.100|x4: 0.000|x5: 0.090|x6: 0.034|x7: 0.000|x8: 0.000|x9: 0.175|x10: 0.126|x11: 0.114|x12: 0.261|x13: 0.100|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.27]</t>
+          <t>[0.00, 0.06, 0.26]</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -4468,7 +4468,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>x1: 0.046|x2: 0.069|x3: 0.101|x4: 0.038|x5: 0.053|x6: 0.047|x7: 0.000|x8: 0.041|x9: 0.075|x10: 0.119|x11: 0.075|x12: 0.077|x13: 0.142|x14: 0.028|x15: 0.048|x16: 0.040|x17: 0.000</t>
+          <t>x1: 0.045|x2: 0.068|x3: 0.099|x4: 0.037|x5: 0.052|x6: 0.046|x7: 0.020|x8: 0.040|x9: 0.074|x10: 0.117|x11: 0.074|x12: 0.075|x13: 0.139|x14: 0.027|x15: 0.047|x16: 0.039|x17: 0.000</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -4550,7 +4550,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>x1: 0.040|x2: 0.056|x3: 0.070|x4: 0.041|x5: 0.054|x6: 0.053|x7: 0.039|x8: 0.049|x9: 0.111|x10: 0.108|x11: 0.101|x12: 0.100|x13: 0.107|x14: 0.030|x15: 0.043|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.039|x2: 0.055|x3: 0.069|x4: 0.040|x5: 0.052|x6: 0.052|x7: 0.038|x8: 0.048|x9: 0.108|x10: 0.106|x11: 0.099|x12: 0.098|x13: 0.104|x14: 0.029|x15: 0.042|x16: 0.020|x17: 0.000</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -4591,12 +4591,12 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>x1: 0.045|x2: 0.045|x3: 0.071|x4: 0.034|x5: 0.064|x6: 0.067|x7: 0.028|x8: 0.075|x9: 0.124|x10: 0.129|x11: 0.078|x12: 0.099|x13: 0.095|x14: 0.000|x15: 0.046|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.044|x2: 0.044|x3: 0.069|x4: 0.033|x5: 0.062|x6: 0.065|x7: 0.027|x8: 0.073|x9: 0.120|x10: 0.125|x11: 0.076|x12: 0.096|x13: 0.092|x14: 0.014|x15: 0.045|x16: 0.015|x17: 0.000</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.13]</t>
+          <t>[0.00, 0.06, 0.12]</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -4796,12 +4796,12 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.087|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.145|x10: 0.209|x11: 0.188|x12: 0.108|x13: 0.264|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.065|x3: 0.044|x4: 0.000|x5: 0.035|x6: 0.036|x7: 0.000|x8: 0.041|x9: 0.108|x10: 0.156|x11: 0.140|x12: 0.080|x13: 0.197|x14: 0.052|x15: 0.045|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.26]</t>
+          <t>[0.00, 0.06, 0.20]</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -4878,12 +4878,12 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.316|x4: 0.000|x5: 0.184|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.172|x13: 0.000|x14: 0.328|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.060|x2: 0.000|x3: 0.164|x4: 0.071|x5: 0.095|x6: 0.059|x7: 0.000|x8: 0.053|x9: 0.074|x10: 0.083|x11: 0.080|x12: 0.089|x13: 0.000|x14: 0.170|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.33]</t>
+          <t>[0.00, 0.06, 0.17]</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -4919,12 +4919,12 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.198|x4: 0.000|x5: 0.124|x6: 0.086|x7: 0.000|x8: 0.000|x9: 0.109|x10: 0.125|x11: 0.121|x12: 0.098|x13: 0.000|x14: 0.139|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.155|x4: 0.063|x5: 0.097|x6: 0.067|x7: 0.000|x8: 0.060|x9: 0.085|x10: 0.098|x11: 0.095|x12: 0.076|x13: 0.061|x14: 0.109|x15: 0.000|x16: 0.034|x17: 0.000</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.20]</t>
+          <t>[0.00, 0.06, 0.15]</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -4960,12 +4960,12 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.112|x3: 0.248|x4: 0.156|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.128|x12: 0.132|x13: 0.000|x14: 0.225|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.059|x2: 0.092|x3: 0.203|x4: 0.128|x5: 0.073|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.046|x10: 0.000|x11: 0.105|x12: 0.108|x13: 0.000|x14: 0.185|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.25]</t>
+          <t>[0.00, 0.06, 0.20]</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -5001,12 +5001,12 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>x1: 0.082|x2: 0.065|x3: 0.127|x4: 0.085|x5: 0.089|x6: 0.062|x7: 0.072|x8: 0.075|x9: 0.083|x10: 0.054|x11: 0.036|x12: 0.040|x13: 0.000|x14: 0.061|x15: 0.068|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.078|x2: 0.063|x3: 0.122|x4: 0.081|x5: 0.086|x6: 0.060|x7: 0.069|x8: 0.072|x9: 0.080|x10: 0.052|x11: 0.035|x12: 0.038|x13: 0.015|x14: 0.058|x15: 0.065|x16: 0.027|x17: 0.000</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.13]</t>
+          <t>[0.00, 0.06, 0.12]</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -5042,22 +5042,22 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.508|x13: 0.000|x14: 0.492|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.090|x4: 0.062|x5: 0.055|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.099|x10: 0.094|x11: 0.102|x12: 0.211|x13: 0.084|x14: 0.204|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.51]</t>
+          <t>[0.00, 0.06, 0.21]</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>[12]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>[0.508360478693156]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H113" t="b">
@@ -5165,12 +5165,12 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.272|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.182|x12: 0.152|x13: 0.000|x14: 0.115|x15: 0.000|x16: 0.280|x17: 0.000</t>
+          <t>x1: 0.068|x2: 0.000|x3: 0.222|x4: 0.054|x5: 0.060|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.148|x12: 0.124|x13: 0.000|x14: 0.094|x15: 0.000|x16: 0.229|x17: 0.000</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.28]</t>
+          <t>[0.00, 0.06, 0.23]</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>x1: 0.083|x2: 0.075|x3: 0.142|x4: 0.070|x5: 0.070|x6: 0.046|x7: 0.054|x8: 0.056|x9: 0.067|x10: 0.035|x11: 0.067|x12: 0.049|x13: 0.000|x14: 0.038|x15: 0.065|x16: 0.084|x17: 0.000</t>
+          <t>x1: 0.082|x2: 0.074|x3: 0.140|x4: 0.069|x5: 0.068|x6: 0.045|x7: 0.053|x8: 0.055|x9: 0.066|x10: 0.035|x11: 0.066|x12: 0.048|x13: 0.015|x14: 0.037|x15: 0.064|x16: 0.082|x17: 0.000</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -5329,12 +5329,12 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>x1: 0.074|x2: 0.045|x3: 0.133|x4: 0.000|x5: 0.059|x6: 0.059|x7: 0.000|x8: 0.058|x9: 0.103|x10: 0.075|x11: 0.113|x12: 0.085|x13: 0.054|x14: 0.000|x15: 0.047|x16: 0.096|x17: 0.000</t>
+          <t>x1: 0.068|x2: 0.041|x3: 0.122|x4: 0.030|x5: 0.054|x6: 0.054|x7: 0.028|x8: 0.053|x9: 0.095|x10: 0.069|x11: 0.104|x12: 0.078|x13: 0.049|x14: 0.024|x15: 0.043|x16: 0.089|x17: 0.000</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.13]</t>
+          <t>[0.00, 0.06, 0.12]</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -5370,12 +5370,12 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>x1: 0.103|x2: 0.077|x3: 0.175|x4: 0.052|x5: 0.082|x6: 0.054|x7: 0.067|x8: 0.065|x9: 0.058|x10: 0.000|x11: 0.000|x12: 0.053|x13: 0.000|x14: 0.042|x15: 0.065|x16: 0.106|x17: 0.000</t>
+          <t>x1: 0.097|x2: 0.072|x3: 0.164|x4: 0.049|x5: 0.077|x6: 0.051|x7: 0.062|x8: 0.061|x9: 0.054|x10: 0.029|x11: 0.033|x12: 0.050|x13: 0.000|x14: 0.040|x15: 0.061|x16: 0.100|x17: 0.000</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.18]</t>
+          <t>[0.00, 0.06, 0.16]</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -5411,12 +5411,12 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>x1: 0.077|x2: 0.041|x3: 0.149|x4: 0.080|x5: 0.088|x6: 0.055|x7: 0.073|x8: 0.058|x9: 0.085|x10: 0.000|x11: 0.075|x12: 0.038|x13: 0.000|x14: 0.085|x15: 0.049|x16: 0.048|x17: 0.000</t>
+          <t>x1: 0.074|x2: 0.040|x3: 0.145|x4: 0.078|x5: 0.085|x6: 0.054|x7: 0.071|x8: 0.056|x9: 0.082|x10: 0.028|x11: 0.072|x12: 0.037|x13: 0.000|x14: 0.083|x15: 0.047|x16: 0.046|x17: 0.000</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.15]</t>
+          <t>[0.00, 0.06, 0.14]</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -5452,12 +5452,12 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>x1: 0.059|x2: 0.066|x3: 0.101|x4: 0.055|x5: 0.077|x6: 0.083|x7: 0.053|x8: 0.128|x9: 0.125|x10: 0.079|x11: 0.079|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.050|x16: 0.044|x17: 0.000</t>
+          <t>x1: 0.055|x2: 0.061|x3: 0.094|x4: 0.051|x5: 0.072|x6: 0.077|x7: 0.049|x8: 0.119|x9: 0.116|x10: 0.074|x11: 0.074|x12: 0.027|x13: 0.021|x14: 0.022|x15: 0.047|x16: 0.041|x17: 0.000</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.13]</t>
+          <t>[0.00, 0.06, 0.12]</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -5534,7 +5534,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>x1: 0.039|x2: 0.148|x3: 0.153|x4: 0.109|x5: 0.059|x6: 0.044|x7: 0.054|x8: 0.037|x9: 0.052|x10: 0.000|x11: 0.087|x12: 0.066|x13: 0.000|x14: 0.038|x15: 0.042|x16: 0.072|x17: 0.000</t>
+          <t>x1: 0.038|x2: 0.146|x3: 0.151|x4: 0.107|x5: 0.058|x6: 0.043|x7: 0.053|x8: 0.036|x9: 0.051|x10: 0.018|x11: 0.085|x12: 0.065|x13: 0.000|x14: 0.038|x15: 0.041|x16: 0.071|x17: 0.000</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
@@ -5657,12 +5657,12 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.143|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.157|x10: 0.178|x11: 0.201|x12: 0.161|x13: 0.161|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.121|x3: 0.000|x4: 0.051|x5: 0.000|x6: 0.051|x7: 0.000|x8: 0.000|x9: 0.133|x10: 0.150|x11: 0.170|x12: 0.136|x13: 0.136|x14: 0.000|x15: 0.054|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.20]</t>
+          <t>[0.00, 0.06, 0.17]</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -5780,12 +5780,12 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>x1: 0.049|x2: 0.053|x3: 0.074|x4: 0.080|x5: 0.121|x6: 0.102|x7: 0.141|x8: 0.146|x9: 0.105|x10: 0.057|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.026|x15: 0.046|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.045|x2: 0.049|x3: 0.069|x4: 0.074|x5: 0.112|x6: 0.095|x7: 0.131|x8: 0.136|x9: 0.098|x10: 0.053|x11: 0.020|x12: 0.014|x13: 0.017|x14: 0.024|x15: 0.043|x16: 0.019|x17: 0.000</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.15]</t>
+          <t>[0.00, 0.06, 0.14]</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -5903,12 +5903,12 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.099|x3: 0.097|x4: 0.083|x5: 0.129|x6: 0.141|x7: 0.073|x8: 0.192|x9: 0.097|x10: 0.087|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.027|x2: 0.087|x3: 0.085|x4: 0.073|x5: 0.112|x6: 0.123|x7: 0.064|x8: 0.168|x9: 0.085|x10: 0.076|x11: 0.029|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.044|x16: 0.026|x17: 0.000</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.19]</t>
+          <t>[0.00, 0.06, 0.17]</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -5985,7 +5985,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>x1: 0.061|x2: 0.067|x3: 0.143|x4: 0.105|x5: 0.089|x6: 0.043|x7: 0.084|x8: 0.063|x9: 0.079|x10: 0.000|x11: 0.043|x12: 0.068|x13: 0.000|x14: 0.107|x15: 0.046|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.058|x2: 0.063|x3: 0.135|x4: 0.100|x5: 0.084|x6: 0.040|x7: 0.080|x8: 0.059|x9: 0.075|x10: 0.030|x11: 0.041|x12: 0.065|x13: 0.000|x14: 0.102|x15: 0.044|x16: 0.024|x17: 0.000</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -6026,7 +6026,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>x1: 0.060|x2: 0.072|x3: 0.105|x4: 0.090|x5: 0.087|x6: 0.071|x7: 0.091|x8: 0.084|x9: 0.087|x10: 0.041|x11: 0.055|x12: 0.033|x13: 0.000|x14: 0.050|x15: 0.052|x16: 0.023|x17: 0.000</t>
+          <t>x1: 0.060|x2: 0.071|x3: 0.104|x4: 0.089|x5: 0.086|x6: 0.071|x7: 0.090|x8: 0.083|x9: 0.086|x10: 0.041|x11: 0.054|x12: 0.032|x13: 0.008|x14: 0.050|x15: 0.051|x16: 0.023|x17: 0.000</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -6067,7 +6067,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>x1: 0.065|x2: 0.067|x3: 0.093|x4: 0.097|x5: 0.129|x6: 0.090|x7: 0.140|x8: 0.126|x9: 0.072|x10: 0.031|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.032|x15: 0.058|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.063|x2: 0.065|x3: 0.090|x4: 0.094|x5: 0.125|x6: 0.087|x7: 0.135|x8: 0.122|x9: 0.070|x10: 0.030|x11: 0.000|x12: 0.014|x13: 0.000|x14: 0.031|x15: 0.056|x16: 0.019|x17: 0.000</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -6149,12 +6149,12 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>x1: 0.052|x2: 0.036|x3: 0.074|x4: 0.000|x5: 0.053|x6: 0.064|x7: 0.000|x8: 0.069|x9: 0.124|x10: 0.131|x11: 0.126|x12: 0.079|x13: 0.107|x14: 0.043|x15: 0.042|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.048|x2: 0.034|x3: 0.069|x4: 0.031|x5: 0.050|x6: 0.059|x7: 0.016|x8: 0.065|x9: 0.116|x10: 0.122|x11: 0.117|x12: 0.073|x13: 0.100|x14: 0.041|x15: 0.040|x16: 0.019|x17: 0.000</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.13]</t>
+          <t>[0.00, 0.06, 0.12]</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -6190,7 +6190,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>x1: 0.051|x2: 0.052|x3: 0.120|x4: 0.080|x5: 0.095|x6: 0.076|x7: 0.063|x8: 0.080|x9: 0.076|x10: 0.051|x11: 0.058|x12: 0.064|x13: 0.000|x14: 0.065|x15: 0.039|x16: 0.030|x17: 0.000</t>
+          <t>x1: 0.051|x2: 0.051|x3: 0.118|x4: 0.078|x5: 0.094|x6: 0.075|x7: 0.062|x8: 0.079|x9: 0.074|x10: 0.050|x11: 0.057|x12: 0.063|x13: 0.016|x14: 0.064|x15: 0.038|x16: 0.029|x17: 0.000</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
@@ -6313,12 +6313,12 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.044|x3: 0.080|x4: 0.037|x5: 0.071|x6: 0.072|x7: 0.000|x8: 0.057|x9: 0.148|x10: 0.122|x11: 0.131|x12: 0.168|x13: 0.072|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.028|x2: 0.041|x3: 0.075|x4: 0.035|x5: 0.066|x6: 0.068|x7: 0.000|x8: 0.054|x9: 0.139|x10: 0.115|x11: 0.123|x12: 0.158|x13: 0.067|x14: 0.000|x15: 0.031|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.17]</t>
+          <t>[0.00, 0.06, 0.16]</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -6354,12 +6354,12 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.063|x3: 0.087|x4: 0.041|x5: 0.076|x6: 0.061|x7: 0.000|x8: 0.033|x9: 0.110|x10: 0.125|x11: 0.085|x12: 0.191|x13: 0.090|x14: 0.000|x15: 0.039|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.019|x2: 0.059|x3: 0.082|x4: 0.039|x5: 0.072|x6: 0.057|x7: 0.000|x8: 0.031|x9: 0.104|x10: 0.118|x11: 0.081|x12: 0.181|x13: 0.085|x14: 0.019|x15: 0.037|x16: 0.017|x17: 0.000</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.19]</t>
+          <t>[0.00, 0.06, 0.18]</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -6395,7 +6395,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>x1: 0.032|x2: 0.073|x3: 0.092|x4: 0.048|x5: 0.065|x6: 0.054|x7: 0.000|x8: 0.042|x9: 0.086|x10: 0.118|x11: 0.088|x12: 0.095|x13: 0.123|x14: 0.038|x15: 0.047|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.030|x2: 0.070|x3: 0.087|x4: 0.046|x5: 0.062|x6: 0.051|x7: 0.025|x8: 0.040|x9: 0.082|x10: 0.112|x11: 0.084|x12: 0.090|x13: 0.117|x14: 0.036|x15: 0.044|x16: 0.025|x17: 0.000</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
@@ -6477,12 +6477,12 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.092|x3: 0.066|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.122|x10: 0.203|x11: 0.117|x12: 0.158|x13: 0.242|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.073|x3: 0.052|x4: 0.026|x5: 0.028|x6: 0.035|x7: 0.000|x8: 0.032|x9: 0.097|x10: 0.161|x11: 0.093|x12: 0.126|x13: 0.192|x14: 0.021|x15: 0.035|x16: 0.029|x17: 0.000</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.24]</t>
+          <t>[0.00, 0.06, 0.19]</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -6559,12 +6559,12 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>x1: 0.070|x2: 0.103|x3: 0.159|x4: 0.118|x5: 0.066|x6: 0.000|x7: 0.060|x8: 0.000|x9: 0.079|x10: 0.000|x11: 0.105|x12: 0.064|x13: 0.000|x14: 0.120|x15: 0.057|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.062|x2: 0.092|x3: 0.142|x4: 0.106|x5: 0.059|x6: 0.020|x7: 0.054|x8: 0.023|x9: 0.071|x10: 0.025|x11: 0.094|x12: 0.057|x13: 0.016|x14: 0.107|x15: 0.050|x16: 0.024|x17: 0.000</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.16]</t>
+          <t>[0.00, 0.06, 0.14]</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -6600,12 +6600,12 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.186|x4: 0.000|x5: 0.129|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.157|x10: 0.131|x11: 0.202|x12: 0.000|x13: 0.000|x14: 0.195|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.047|x2: 0.000|x3: 0.123|x4: 0.071|x5: 0.086|x6: 0.054|x7: 0.000|x8: 0.053|x9: 0.104|x10: 0.087|x11: 0.134|x12: 0.064|x13: 0.048|x14: 0.129|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.20]</t>
+          <t>[0.00, 0.06, 0.13]</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">

</xml_diff>